<commit_message>
客户端： [CMessage]增加是，否，另存为按钮、外部传入文件名 [public]switch格式规范，static_cast强转unsigned long long 增加json字段解析transferfilerequest、transferfilerespond、transferfile [chatclient]界面增加文件接受框，文件传输线程，LOGINBOARDCAST传输更改，TRANSFERFILEREQUEST消息
</commit_message>
<xml_diff>
--- a/网络聊天室测试.xlsx
+++ b/网络聊天室测试.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <t>网络聊天室测试</t>
   </si>
@@ -54,10 +54,11 @@
     <t>注册用户</t>
   </si>
   <si>
-    <t>用户：aaa，密码：aaa</t>
-  </si>
-  <si>
-    <t>客户端：{ "communication_type":"register", "customer" : "aaa", "password" : "aaa"}</t>
+    <t>用户：藐视①切，密码：Chen590526</t>
+  </si>
+  <si>
+    <t>客户端：{ "communication_type":"register", "customer" : "藐视①切", 
+"password" : "Chen500526"}</t>
   </si>
   <si>
     <t>服务器：{"communication_type":"registerbacksucceed","id":"10001","register_result":"succeed"}</t>
@@ -75,10 +76,10 @@
     <t>用户登录</t>
   </si>
   <si>
-    <t>用户：aaa，密码：ccc</t>
-  </si>
-  <si>
-    <t>客户端：{ "communication_type":"login", "customer" : "aaa", "password" : "ccc"}</t>
+    <t>id：10001，密码：ccc</t>
+  </si>
+  <si>
+    <t>客户端：{ "communication_type":"login", "id" : "10001", "password" : "ccc"}</t>
   </si>
   <si>
     <t>服务器：{"communication_type":"loginbackfailed","customer":"aaa",
@@ -88,7 +89,10 @@
     <t>登录失败</t>
   </si>
   <si>
-    <t>客户端：{ "communication_type":"login", "customer" : "aaa", "password" : "aaa"}</t>
+    <t>id：10001，密码：aaa</t>
+  </si>
+  <si>
+    <t>客户端：{ "communication_type":"login", "id" : "10001", "password" : "aaa"}</t>
   </si>
   <si>
     <t>服务器：{"communication_type":"loginbacksucceed","customer":"aaa","login_result":"succeed"}</t>
@@ -97,10 +101,10 @@
     <t>成功登录</t>
   </si>
   <si>
-    <t>用户：ccc，密码：ccc</t>
-  </si>
-  <si>
-    <t>客户端：{ "communication_type":"login", "customer" : "ccc", "password" : "ccc"}</t>
+    <t>id：20000，密码：ccc</t>
+  </si>
+  <si>
+    <t>客户端：{ "communication_type":"login", "id" : "20000", "password" : "ccc"}</t>
   </si>
   <si>
     <t>服务器：{"communication_type":"loginbackfailed","customer":"ccc",
@@ -113,16 +117,24 @@
     <t>显示登录</t>
   </si>
   <si>
+    <t>用户10002登录</t>
+  </si>
+  <si>
+    <t>服务器-》10001：{"communication_type":"loginboardcast",
+"customer":"赤眼の沙萨-127.0.0.1"}</t>
+  </si>
+  <si>
+    <t>服务器-》10002：{"communication_type":"loginboardcast",
+"customer":"aaa-127.0.0.1"}</t>
+  </si>
+  <si>
+    <t>deletecustomer</t>
+  </si>
+  <si>
+    <t>用户退出</t>
+  </si>
+  <si>
     <t>用户：aaa</t>
-  </si>
-  <si>
-    <t>服务器：{"communication_type":"loginboardcast","customer":"aaa-127.0.0.1"}</t>
-  </si>
-  <si>
-    <t>deletecustomer</t>
-  </si>
-  <si>
-    <t>用户退出</t>
   </si>
   <si>
     <t>客户端：{ "communication_type":"delcustomer", "customer" : "aaa"}</t>
@@ -160,7 +172,7 @@
     <t>target：{ "communication_type":"chat", "source" : "aaa", "target" : "bbb", "content" : "Hello"}</t>
   </si>
   <si>
-    <t>transferfile</t>
+    <t>transferfilerequest</t>
   </si>
   <si>
     <t>传送文件</t>
@@ -181,9 +193,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -209,6 +221,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -217,14 +244,70 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,76 +321,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -316,16 +329,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -340,7 +352,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,13 +367,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,169 +529,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,6 +674,15 @@
       <top/>
       <bottom style="thick">
         <color rgb="FF00B050"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -681,11 +702,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,50 +756,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -771,10 +783,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -786,30 +798,33 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -819,101 +834,98 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -950,6 +962,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -967,6 +982,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1325,12 +1343,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T94"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="D17" sqref="D17"/>
+      <selection pane="topRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1356,18 +1374,18 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
     </row>
     <row r="2" ht="15" spans="1:8">
       <c r="A2" s="4" t="s">
@@ -1393,7 +1411,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" ht="15" spans="1:8">
+    <row r="3" spans="1:8">
       <c r="A3" s="8"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1407,7 +1425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" ht="15" spans="1:8">
+    <row r="4" ht="28.5" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1435,7 @@
       <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -1444,7 +1462,7 @@
       <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="9" t="s">
@@ -1456,172 +1474,184 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" ht="27.75" spans="1:8">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="E7" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="18"/>
     </row>
-    <row r="8" ht="15" spans="1:8">
+    <row r="8" ht="28.5" spans="1:8">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" ht="15" spans="1:8">
-      <c r="A9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="5" t="s">
+    <row r="9" ht="28.5" spans="1:8">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" ht="27.75" spans="1:8">
-      <c r="A10" s="8" t="s">
+    <row r="10" ht="15" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="E10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="F10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" ht="27.75" spans="1:8">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15" t="s">
+      <c r="A11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="17"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
     </row>
-    <row r="12" ht="14.25" spans="1:8">
-      <c r="A12" s="8" t="s">
+    <row r="12" ht="27.75" spans="1:8">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="D12" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="E12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="18"/>
     </row>
-    <row r="13" ht="27" customHeight="1" spans="1:8">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
+    <row r="13" ht="14.25" spans="1:8">
+      <c r="A13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="B13" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="17"/>
+      <c r="C13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
     </row>
-    <row r="14" ht="14.25"/>
-    <row r="16" spans="1:8">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+    <row r="14" ht="27" customHeight="1" spans="1:8">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="18"/>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="19"/>
+    <row r="15" ht="14.25"/>
+    <row r="17" spans="1:8">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="L5:Q94"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="L5:Q95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>